<commit_message>
flops resource allocation including evaluation steps
</commit_message>
<xml_diff>
--- a/LoRA_FLOPs_plan.xlsx
+++ b/LoRA_FLOPs_plan.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raunaqrai/Documents/DIS/m2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42048E13-B61D-364A-A2ED-01C0535FF1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B2BF94-C133-924C-814F-C4DDC825D2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="21580" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3220" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Part</t>
   </si>
@@ -80,6 +93,18 @@
   </si>
   <si>
     <t>Best</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Budget</t>
+  </si>
+  <si>
+    <t>* no 512 since already done</t>
+  </si>
+  <si>
+    <t>max training steps</t>
   </si>
 </sst>
 </file>
@@ -138,11 +163,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,24 +473,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,36 +520,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>1E-4</v>
       </c>
-      <c r="E2">
-        <v>512</v>
-      </c>
-      <c r="F2">
-        <v>4000</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
+      <c r="E3">
+        <v>512</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
         <v>16.440000000000001</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>65760</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -538,9 +565,6 @@
       <c r="E5">
         <v>512</v>
       </c>
-      <c r="F5">
-        <v>1000</v>
-      </c>
       <c r="G5">
         <v>4</v>
       </c>
@@ -551,7 +575,7 @@
         <v>4110</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -568,7 +592,7 @@
         <v>512</v>
       </c>
       <c r="F6">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -580,7 +604,7 @@
         <v>6165.0000000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -596,9 +620,6 @@
       <c r="E7">
         <v>512</v>
       </c>
-      <c r="F7">
-        <v>1000</v>
-      </c>
       <c r="G7">
         <v>4</v>
       </c>
@@ -609,7 +630,7 @@
         <v>4110</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -626,7 +647,7 @@
         <v>512</v>
       </c>
       <c r="F8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -638,7 +659,7 @@
         <v>12330</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -655,7 +676,7 @@
         <v>512</v>
       </c>
       <c r="F9">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -667,7 +688,7 @@
         <v>12330</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -684,7 +705,7 @@
         <v>512</v>
       </c>
       <c r="F10">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -696,7 +717,7 @@
         <v>12330</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -712,9 +733,6 @@
       <c r="E11">
         <v>512</v>
       </c>
-      <c r="F11">
-        <v>1000</v>
-      </c>
       <c r="G11">
         <v>4</v>
       </c>
@@ -725,7 +743,7 @@
         <v>16440</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -742,7 +760,7 @@
         <v>512</v>
       </c>
       <c r="F12">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G12">
         <v>4</v>
@@ -754,7 +772,7 @@
         <v>24660</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -770,9 +788,6 @@
       <c r="E13">
         <v>512</v>
       </c>
-      <c r="F13">
-        <v>1500</v>
-      </c>
       <c r="G13">
         <v>4</v>
       </c>
@@ -783,7 +798,7 @@
         <v>24660</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -811,8 +826,11 @@
       <c r="I14">
         <v>24660</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -841,7 +859,7 @@
         <v>36990</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -858,7 +876,7 @@
         <v>512</v>
       </c>
       <c r="F18">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="G18">
         <v>4</v>
@@ -870,7 +888,7 @@
         <v>49320.000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -880,9 +898,6 @@
       <c r="E21">
         <v>512</v>
       </c>
-      <c r="F21">
-        <v>5000</v>
-      </c>
       <c r="G21">
         <v>1</v>
       </c>
@@ -893,7 +908,7 @@
         <v>27400</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -903,9 +918,6 @@
       <c r="E22">
         <v>512</v>
       </c>
-      <c r="F22">
-        <v>5000</v>
-      </c>
       <c r="G22">
         <v>1</v>
       </c>
@@ -914,6 +926,35 @@
       </c>
       <c r="I22">
         <v>27400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <f>SUM(F3:F22)</f>
+        <v>11000</v>
+      </c>
+      <c r="I24">
+        <f>SUM(I3:I22)</f>
+        <v>348665</v>
+      </c>
+      <c r="K24">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="2">
+        <v>14776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>